<commit_message>
Fix example and more codacy issues
</commit_message>
<xml_diff>
--- a/examples/databases/dtocean-maintenance/multiplehubs.xlsx
+++ b/examples/databases/dtocean-maintenance/multiplehubs.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{077ECFBF-0C78-4A79-8955-DC2CBDF1B409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="28830" windowHeight="4280" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Components" sheetId="1" r:id="rId1"/>
@@ -12,12 +13,23 @@
     <sheet name="RepairActions" sheetId="4" r:id="rId3"/>
     <sheet name="Inspections" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="55">
   <si>
     <t>False</t>
   </si>
@@ -179,12 +191,15 @@
   </si>
   <si>
     <t>CAPEX_condition_based_maintenance [Euro]</t>
+  </si>
+  <si>
+    <t>Export cable</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -376,6 +391,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -411,6 +443,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -586,24 +635,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" customWidth="1"/>
-    <col min="2" max="13" width="20.1796875" customWidth="1"/>
-    <col min="14" max="14" width="18.26953125" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" customWidth="1"/>
+    <col min="2" max="13" width="20.140625" customWidth="1"/>
+    <col min="14" max="14" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="7" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" s="7" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -644,7 +693,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10">
         <v>1</v>
       </c>
@@ -682,7 +731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
         <v>2</v>
       </c>
@@ -690,10 +739,10 @@
         <v>50</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="E3" s="10">
         <f>1/15</f>
@@ -720,7 +769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
         <v>3</v>
       </c>
@@ -731,7 +780,7 @@
         <v>51</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="E4" s="10">
         <f>1/15</f>
@@ -758,7 +807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -781,7 +830,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -791,18 +840,18 @@
       <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.7265625" customWidth="1"/>
-    <col min="3" max="3" width="19.7265625" customWidth="1"/>
-    <col min="4" max="4" width="12.1796875" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="12" width="14.54296875" customWidth="1"/>
-    <col min="13" max="13" width="16.1796875" customWidth="1"/>
-    <col min="14" max="14" width="14.54296875" customWidth="1"/>
+    <col min="6" max="12" width="14.5703125" customWidth="1"/>
+    <col min="13" max="13" width="16.140625" customWidth="1"/>
+    <col min="14" max="14" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="9" customFormat="1" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" s="9" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
@@ -843,7 +892,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10">
         <v>1</v>
       </c>
@@ -884,7 +933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
         <v>2</v>
       </c>
@@ -925,7 +974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
         <v>3</v>
       </c>
@@ -967,13 +1016,13 @@
       </c>
       <c r="N4" s="1"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="N5" s="1"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M6" s="4"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M7" s="4"/>
     </row>
   </sheetData>
@@ -984,25 +1033,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:X4"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S2" sqref="S2:S4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.54296875" customWidth="1"/>
-    <col min="2" max="2" width="21.453125" customWidth="1"/>
-    <col min="3" max="22" width="11.54296875" customWidth="1"/>
+    <col min="1" max="1" width="8.5703125" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" customWidth="1"/>
+    <col min="3" max="22" width="11.5703125" customWidth="1"/>
     <col min="23" max="23" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="7" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:24" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -1070,7 +1119,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10">
         <v>1</v>
       </c>
@@ -1138,7 +1187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
         <v>2</v>
       </c>
@@ -1206,7 +1255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
         <v>3</v>
       </c>
@@ -1284,27 +1333,27 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.81640625" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="7.26953125" customWidth="1"/>
-    <col min="5" max="5" width="10.54296875" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
-    <col min="7" max="7" width="6.54296875" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="7" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:19" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -1363,7 +1412,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improve calculation efficiency and integration with RAM  (#4)
* Change om_logistics_main function to Logistics class to reduce repetitive initialisation

* Use Logistics class to hold logisitcs object and avoid costly initialisation and recalculation

* Remove excessive use of Dataframe appending using loc

* Remove costly call to DataFrame.sort_values

* Fix case where no calendar based events are scheduled

* Remove unused ComponentIDLogistic variable

* Add logging of selected ports

* Move some log messages to DEBUG level

* Integrate new RAM module

* Remove comparisons with nan

* Allow kfactor calculation for static cable reliability

* Pass precomputed kfactors directly.

* Add logging setup function and get version from setup.py

* Use appveyor config as single source of truth
</commit_message>
<xml_diff>
--- a/examples/databases/dtocean-maintenance/multiplehubs.xlsx
+++ b/examples/databases/dtocean-maintenance/multiplehubs.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{077ECFBF-0C78-4A79-8955-DC2CBDF1B409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="28830" windowHeight="4280" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Components" sheetId="1" r:id="rId1"/>
@@ -12,12 +13,23 @@
     <sheet name="RepairActions" sheetId="4" r:id="rId3"/>
     <sheet name="Inspections" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="55">
   <si>
     <t>False</t>
   </si>
@@ -179,12 +191,15 @@
   </si>
   <si>
     <t>CAPEX_condition_based_maintenance [Euro]</t>
+  </si>
+  <si>
+    <t>Export cable</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -376,6 +391,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -411,6 +443,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -586,24 +635,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" customWidth="1"/>
-    <col min="2" max="13" width="20.1796875" customWidth="1"/>
-    <col min="14" max="14" width="18.26953125" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" customWidth="1"/>
+    <col min="2" max="13" width="20.140625" customWidth="1"/>
+    <col min="14" max="14" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="7" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" s="7" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -644,7 +693,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10">
         <v>1</v>
       </c>
@@ -682,7 +731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
         <v>2</v>
       </c>
@@ -690,10 +739,10 @@
         <v>50</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="E3" s="10">
         <f>1/15</f>
@@ -720,7 +769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
         <v>3</v>
       </c>
@@ -731,7 +780,7 @@
         <v>51</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="E4" s="10">
         <f>1/15</f>
@@ -758,7 +807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -781,7 +830,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -791,18 +840,18 @@
       <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.7265625" customWidth="1"/>
-    <col min="3" max="3" width="19.7265625" customWidth="1"/>
-    <col min="4" max="4" width="12.1796875" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="12" width="14.54296875" customWidth="1"/>
-    <col min="13" max="13" width="16.1796875" customWidth="1"/>
-    <col min="14" max="14" width="14.54296875" customWidth="1"/>
+    <col min="6" max="12" width="14.5703125" customWidth="1"/>
+    <col min="13" max="13" width="16.140625" customWidth="1"/>
+    <col min="14" max="14" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="9" customFormat="1" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" s="9" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
@@ -843,7 +892,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10">
         <v>1</v>
       </c>
@@ -884,7 +933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
         <v>2</v>
       </c>
@@ -925,7 +974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
         <v>3</v>
       </c>
@@ -967,13 +1016,13 @@
       </c>
       <c r="N4" s="1"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="N5" s="1"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M6" s="4"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M7" s="4"/>
     </row>
   </sheetData>
@@ -984,25 +1033,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:X4"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S2" sqref="S2:S4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.54296875" customWidth="1"/>
-    <col min="2" max="2" width="21.453125" customWidth="1"/>
-    <col min="3" max="22" width="11.54296875" customWidth="1"/>
+    <col min="1" max="1" width="8.5703125" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" customWidth="1"/>
+    <col min="3" max="22" width="11.5703125" customWidth="1"/>
     <col min="23" max="23" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="7" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:24" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -1070,7 +1119,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10">
         <v>1</v>
       </c>
@@ -1138,7 +1187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
         <v>2</v>
       </c>
@@ -1206,7 +1255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
         <v>3</v>
       </c>
@@ -1284,27 +1333,27 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.81640625" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="7.26953125" customWidth="1"/>
-    <col min="5" max="5" width="10.54296875" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
-    <col min="7" max="7" width="6.54296875" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="7" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:19" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -1363,7 +1412,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="3"/>
     </row>
   </sheetData>

</xml_diff>